<commit_message>
update import excel to create user
</commit_message>
<xml_diff>
--- a/FontEnd/pc3-edu-fontend/public/Excel/Users.xlsx
+++ b/FontEnd/pc3-edu-fontend/public/Excel/Users.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Ngôi nhà</t>
-  </si>
-  <si>
-    <t>House</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>fullname</t>
   </si>
@@ -54,6 +48,21 @@
   </si>
   <si>
     <t>Học sinh</t>
+  </si>
+  <si>
+    <t>0358489850</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn A</t>
+  </si>
+  <si>
+    <t>vana12a1@gmail.com</t>
+  </si>
+  <si>
+    <t>Phù Cát, Bình Định</t>
+  </si>
+  <si>
+    <t>12A1</t>
   </si>
 </sst>
 </file>
@@ -61,9 +70,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +84,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,10 +147,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,14 +165,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,13 +467,13 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="26.44140625" customWidth="1"/>
     <col min="5" max="5" width="23.109375" customWidth="1"/>
@@ -452,51 +483,57 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" s="5">
-        <v>44196</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>43908</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="10"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -743,16 +780,27 @@
       <c r="G30" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C30">
+  <dataConsolidate/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"Quản trị viên, Giáo Viên, Học sinh"</formula1>
     </dataValidation>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo lỗi!" error="Ngày sinh không đúng định dạng vui lòng kiểm tra lại!" sqref="E2:E30">
       <formula1>16438</formula1>
       <formula2>54789</formula2>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Thông Báo!" error="Bạn chỉ được chọn 1 trong 3 chức vụ._x000a_Học sinh, Quản trị viên, Giáo viên" sqref="C3:C30">
+      <formula1>"Quản trị viên, Giáo Viên, Học sinh"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Thông Báo!" error="Số điện thoại chỉ bao gồm 10 hoặc 11 số" sqref="F2">
+      <formula1>0</formula1>
+      <formula2>11</formula2>
+    </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>